<commit_message>
finishing delay to admission section
</commit_message>
<xml_diff>
--- a/write/tables/tb_model_accept_all_sims100.xlsx
+++ b/write/tables/tb_model_accept_all_sims100.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="12000" yWindow="460" windowWidth="16800" windowHeight="17460" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="14400" yWindow="460" windowWidth="14400" windowHeight="17460" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="readme" sheetId="8" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="281">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="282">
   <si>
     <t>V1</t>
   </si>
@@ -873,6 +873,9 @@
   </si>
   <si>
     <t>Hospital level variation</t>
+  </si>
+  <si>
+    <t>Reference</t>
   </si>
 </sst>
 </file>
@@ -882,7 +885,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="mm/dd/yyyy\ hh:mm:ss"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -923,6 +926,12 @@
       <color rgb="FF000000"/>
       <name val="Times New Roman"/>
     </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Times New Roman"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -961,7 +970,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="22">
+  <cellStyleXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0">
       <alignment wrapText="1"/>
@@ -994,8 +1003,16 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1024,9 +1041,6 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1043,8 +1057,37 @@
     <xf numFmtId="2" fontId="4" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="22">
+  <cellStyles count="30">
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="11" builtinId="9" hidden="1"/>
@@ -1053,6 +1096,10 @@
     <cellStyle name="Followed Hyperlink" xfId="17" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="19" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="21" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="23" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="25" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="27" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="29" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="8" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="10" builtinId="8" hidden="1"/>
@@ -1061,6 +1108,10 @@
     <cellStyle name="Hyperlink" xfId="16" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="18" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="20" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="22" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="24" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="26" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="28" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="XLConnect.Boolean" xfId="4"/>
     <cellStyle name="XLConnect.DateTime" xfId="5"/>
@@ -1353,10 +1404,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:I30"/>
+  <dimension ref="B3:I31"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="J23" sqref="J23"/>
+      <selection activeCell="J32" sqref="A1:J32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -1433,10 +1484,10 @@
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.15">
       <c r="C5" s="9"/>
-      <c r="D5" s="14" t="s">
+      <c r="D5" s="20" t="s">
         <v>276</v>
       </c>
-      <c r="E5" s="14"/>
+      <c r="E5" s="20"/>
       <c r="F5" s="11" t="s">
         <v>277</v>
       </c>
@@ -1485,18 +1536,18 @@
         <f>results!A4</f>
         <v>weekend</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="7" t="s">
         <v>255</v>
       </c>
-      <c r="D8" s="10" t="str">
+      <c r="D8" s="12" t="str">
         <f>results!B4</f>
         <v>1.15</v>
       </c>
-      <c r="E8" s="1" t="str">
+      <c r="E8" s="6" t="str">
         <f>results!C4</f>
         <v>(1.04--1.27)</v>
       </c>
-      <c r="F8" s="10" t="str">
+      <c r="F8" s="12" t="str">
         <f>results!D4</f>
         <v>0.006</v>
       </c>
@@ -1558,9 +1609,11 @@
       <c r="C11" s="7" t="s">
         <v>257</v>
       </c>
-      <c r="D11" s="12"/>
-      <c r="E11" s="6"/>
-      <c r="F11" s="12"/>
+      <c r="D11" s="22" t="s">
+        <v>281</v>
+      </c>
+      <c r="E11" s="22"/>
+      <c r="F11" s="22"/>
     </row>
     <row r="12" spans="2:9" x14ac:dyDescent="0.15">
       <c r="B12" s="1" t="str">
@@ -1637,6 +1690,11 @@
       <c r="C15" s="3" t="s">
         <v>261</v>
       </c>
+      <c r="D15" s="21" t="s">
+        <v>281</v>
+      </c>
+      <c r="E15" s="21"/>
+      <c r="F15" s="21"/>
     </row>
     <row r="16" spans="2:9" x14ac:dyDescent="0.15">
       <c r="B16" s="1" t="str">
@@ -1742,18 +1800,18 @@
         <f>results!A11</f>
         <v>male</v>
       </c>
-      <c r="C19" s="3" t="s">
+      <c r="C19" s="8" t="s">
         <v>266</v>
       </c>
-      <c r="D19" s="10" t="str">
+      <c r="D19" s="12" t="str">
         <f>results!B11</f>
         <v>1.02</v>
       </c>
-      <c r="E19" s="1" t="str">
+      <c r="E19" s="6" t="str">
         <f>results!C11</f>
         <v>(0.94--1.12)</v>
       </c>
-      <c r="F19" s="10" t="str">
+      <c r="F19" s="12" t="str">
         <f>results!D11</f>
         <v>0.592</v>
       </c>
@@ -1771,38 +1829,40 @@
       </c>
     </row>
     <row r="20" spans="2:9" x14ac:dyDescent="0.15">
-      <c r="C20" s="8" t="s">
+      <c r="C20" s="26" t="s">
         <v>267</v>
       </c>
-      <c r="D20" s="12"/>
-      <c r="E20" s="6"/>
-      <c r="F20" s="12"/>
+      <c r="D20" s="27"/>
+      <c r="E20" s="28"/>
+      <c r="F20" s="27"/>
     </row>
     <row r="21" spans="2:9" x14ac:dyDescent="0.15">
-      <c r="C21" s="7" t="s">
+      <c r="C21" s="29" t="s">
         <v>268</v>
       </c>
-      <c r="D21" s="12"/>
-      <c r="E21" s="6"/>
-      <c r="F21" s="12"/>
+      <c r="D21" s="30" t="s">
+        <v>281</v>
+      </c>
+      <c r="E21" s="30"/>
+      <c r="F21" s="30"/>
     </row>
     <row r="22" spans="2:9" x14ac:dyDescent="0.15">
       <c r="B22" s="1" t="str">
         <f>results!A12</f>
         <v>sepsis_dx1</v>
       </c>
-      <c r="C22" s="7" t="s">
+      <c r="C22" s="29" t="s">
         <v>269</v>
       </c>
-      <c r="D22" s="12" t="str">
+      <c r="D22" s="27" t="str">
         <f>results!B12</f>
         <v>1.12</v>
       </c>
-      <c r="E22" s="6" t="str">
+      <c r="E22" s="28" t="str">
         <f>results!C12</f>
         <v>(0.98--1.30)</v>
       </c>
-      <c r="F22" s="12" t="str">
+      <c r="F22" s="27" t="str">
         <f>results!D12</f>
         <v>0.103</v>
       </c>
@@ -1824,18 +1884,18 @@
         <f>results!A13</f>
         <v>sepsis_dx2</v>
       </c>
-      <c r="C23" s="7" t="s">
+      <c r="C23" s="29" t="s">
         <v>270</v>
       </c>
-      <c r="D23" s="12" t="str">
+      <c r="D23" s="27" t="str">
         <f>results!B13</f>
         <v>1.11</v>
       </c>
-      <c r="E23" s="6" t="str">
+      <c r="E23" s="28" t="str">
         <f>results!C13</f>
         <v>(0.92--1.34)</v>
       </c>
-      <c r="F23" s="12" t="str">
+      <c r="F23" s="27" t="str">
         <f>results!D13</f>
         <v>0.262</v>
       </c>
@@ -1857,18 +1917,18 @@
         <f>results!A14</f>
         <v>sepsis_dx3</v>
       </c>
-      <c r="C24" s="7" t="s">
+      <c r="C24" s="29" t="s">
         <v>271</v>
       </c>
-      <c r="D24" s="12" t="str">
+      <c r="D24" s="27" t="str">
         <f>results!B14</f>
         <v>1.37</v>
       </c>
-      <c r="E24" s="6" t="str">
+      <c r="E24" s="28" t="str">
         <f>results!C14</f>
         <v>(1.18--1.59)</v>
       </c>
-      <c r="F24" s="12" t="str">
+      <c r="F24" s="27" t="str">
         <f>results!D14</f>
         <v>&lt;0.001</v>
       </c>
@@ -1890,18 +1950,18 @@
         <f>results!A15</f>
         <v>sepsis_dx4</v>
       </c>
-      <c r="C25" s="7" t="s">
+      <c r="C25" s="29" t="s">
         <v>272</v>
       </c>
-      <c r="D25" s="12" t="str">
+      <c r="D25" s="27" t="str">
         <f>results!B15</f>
         <v>1.25</v>
       </c>
-      <c r="E25" s="6" t="str">
+      <c r="E25" s="28" t="str">
         <f>results!C15</f>
         <v>(1.12--1.40)</v>
       </c>
-      <c r="F25" s="12" t="str">
+      <c r="F25" s="27" t="str">
         <f>results!D15</f>
         <v>&lt;0.001</v>
       </c>
@@ -1923,18 +1983,18 @@
         <f>results!A16</f>
         <v>osupp2</v>
       </c>
-      <c r="C26" s="3" t="s">
+      <c r="C26" s="8" t="s">
         <v>273</v>
       </c>
-      <c r="D26" s="10" t="str">
+      <c r="D26" s="12" t="str">
         <f>results!B16</f>
         <v>1.83</v>
       </c>
-      <c r="E26" s="1" t="str">
+      <c r="E26" s="6" t="str">
         <f>results!C16</f>
         <v>(1.55--2.16)</v>
       </c>
-      <c r="F26" s="10" t="str">
+      <c r="F26" s="12" t="str">
         <f>results!D16</f>
         <v>&lt;0.001</v>
       </c>
@@ -1956,7 +2016,7 @@
         <f>results!A17</f>
         <v>icnarc_score</v>
       </c>
-      <c r="C27" s="3" t="s">
+      <c r="C27" s="4" t="s">
         <v>274</v>
       </c>
       <c r="D27" s="10" t="str">
@@ -1989,18 +2049,18 @@
         <f>results!A18</f>
         <v>periarrest</v>
       </c>
-      <c r="C28" s="16" t="s">
+      <c r="C28" s="23" t="s">
         <v>275</v>
       </c>
-      <c r="D28" s="17" t="str">
+      <c r="D28" s="24" t="str">
         <f>results!B18</f>
         <v>6.32</v>
       </c>
-      <c r="E28" s="18" t="str">
+      <c r="E28" s="25" t="str">
         <f>results!C18</f>
         <v>(5.18--7.70)</v>
       </c>
-      <c r="F28" s="17" t="str">
+      <c r="F28" s="24" t="str">
         <f>results!D18</f>
         <v>&lt;0.001</v>
       </c>
@@ -2018,30 +2078,39 @@
       </c>
     </row>
     <row r="29" spans="2:9" x14ac:dyDescent="0.15">
-      <c r="C29" s="6" t="s">
+      <c r="C29" s="15"/>
+      <c r="D29" s="16"/>
+      <c r="E29" s="17"/>
+      <c r="F29" s="16"/>
+    </row>
+    <row r="30" spans="2:9" x14ac:dyDescent="0.15">
+      <c r="C30" s="6" t="s">
         <v>280</v>
       </c>
-      <c r="D29" s="12"/>
-      <c r="E29" s="6"/>
-      <c r="F29" s="12"/>
-    </row>
-    <row r="30" spans="2:9" x14ac:dyDescent="0.15">
-      <c r="C30" s="19" t="s">
+      <c r="D30" s="12"/>
+      <c r="E30" s="6"/>
+      <c r="F30" s="12"/>
+    </row>
+    <row r="31" spans="2:9" x14ac:dyDescent="0.15">
+      <c r="C31" s="18" t="s">
         <v>279</v>
       </c>
-      <c r="D30" s="20">
+      <c r="D31" s="19">
         <f>VALUE(boot!B2)</f>
         <v>2.1055545046014399</v>
       </c>
-      <c r="E30" s="19" t="str">
+      <c r="E31" s="18" t="str">
         <f>CONCATENATE("(",ROUND(VALUE(boot!C2),2),"--",ROUND(VALUE(boot!D2),2),")")</f>
         <v>(1.81--2.42)</v>
       </c>
-      <c r="F30" s="19"/>
+      <c r="F31" s="18"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="4">
     <mergeCell ref="D5:E5"/>
+    <mergeCell ref="D11:F11"/>
+    <mergeCell ref="D15:F15"/>
+    <mergeCell ref="D21:F21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -2060,7 +2129,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1" ht="105" x14ac:dyDescent="0.2">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="14" t="s">
         <v>278</v>
       </c>
     </row>

</xml_diff>

<commit_message>
excel tables all updated
</commit_message>
<xml_diff>
--- a/write/tables/tb_model_accept_all_sims100.xlsx
+++ b/write/tables/tb_model_accept_all_sims100.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="14400" yWindow="460" windowWidth="14400" windowHeight="17460" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="16800" yWindow="460" windowWidth="16800" windowHeight="20460" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="readme" sheetId="8" r:id="rId1"/>
@@ -970,7 +970,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="30">
+  <cellStyleXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0">
       <alignment wrapText="1"/>
@@ -1011,8 +1011,14 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1057,15 +1063,6 @@
     <xf numFmtId="2" fontId="4" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1083,11 +1080,27 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="30">
+  <cellStyles count="36">
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="11" builtinId="9" hidden="1"/>
@@ -1100,6 +1113,9 @@
     <cellStyle name="Followed Hyperlink" xfId="25" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="27" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="29" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="31" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="33" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="35" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="8" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="10" builtinId="8" hidden="1"/>
@@ -1112,6 +1128,9 @@
     <cellStyle name="Hyperlink" xfId="24" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="26" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="28" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="30" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="32" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="34" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="XLConnect.Boolean" xfId="4"/>
     <cellStyle name="XLConnect.DateTime" xfId="5"/>
@@ -1404,10 +1423,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:I31"/>
+  <dimension ref="B3:I32"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="J32" sqref="A1:J32"/>
+      <selection activeCell="F28" sqref="F28:F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -1484,633 +1503,639 @@
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.15">
       <c r="C5" s="9"/>
-      <c r="D5" s="20" t="s">
+      <c r="D5" s="27" t="s">
         <v>276</v>
       </c>
-      <c r="E5" s="20"/>
+      <c r="E5" s="27"/>
       <c r="F5" s="11" t="s">
         <v>277</v>
       </c>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.15">
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="4" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="7" spans="2:9" x14ac:dyDescent="0.15">
+      <c r="C7" s="3" t="s">
+        <v>261</v>
+      </c>
+      <c r="D7" s="29" t="s">
+        <v>281</v>
+      </c>
+      <c r="E7" s="29"/>
+      <c r="F7" s="29"/>
+    </row>
+    <row r="8" spans="2:9" x14ac:dyDescent="0.15">
+      <c r="B8" s="1" t="str">
+        <f>results!A8</f>
+        <v>age_k1</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>262</v>
+      </c>
+      <c r="D8" s="10" t="str">
+        <f>results!B8</f>
+        <v>0.89</v>
+      </c>
+      <c r="E8" s="1" t="str">
+        <f>results!C8</f>
+        <v>(0.76--1.04)</v>
+      </c>
+      <c r="F8" s="10" t="str">
+        <f>results!D8</f>
+        <v>0.152</v>
+      </c>
+      <c r="G8" s="1" t="str">
+        <f>results!E8</f>
+        <v/>
+      </c>
+      <c r="H8" s="1" t="str">
+        <f>results!F8</f>
+        <v>0.76</v>
+      </c>
+      <c r="I8" s="1" t="str">
+        <f>results!G8</f>
+        <v>1.04</v>
+      </c>
+    </row>
+    <row r="9" spans="2:9" x14ac:dyDescent="0.15">
+      <c r="B9" s="1" t="str">
+        <f>results!A9</f>
+        <v>age_k2</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>263</v>
+      </c>
+      <c r="D9" s="10" t="str">
+        <f>results!B9</f>
+        <v>0.76</v>
+      </c>
+      <c r="E9" s="1" t="str">
+        <f>results!C9</f>
+        <v>(0.66--0.89)</v>
+      </c>
+      <c r="F9" s="10" t="str">
+        <f>results!D9</f>
+        <v>&lt;0.001</v>
+      </c>
+      <c r="G9" s="1" t="str">
+        <f>results!E9</f>
+        <v>***</v>
+      </c>
+      <c r="H9" s="1" t="str">
+        <f>results!F9</f>
+        <v>0.66</v>
+      </c>
+      <c r="I9" s="1" t="str">
+        <f>results!G9</f>
+        <v>0.89</v>
+      </c>
+    </row>
+    <row r="10" spans="2:9" x14ac:dyDescent="0.15">
+      <c r="B10" s="1" t="str">
+        <f>results!A10</f>
+        <v>age_k3</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>264</v>
+      </c>
+      <c r="D10" s="10" t="str">
+        <f>results!B10</f>
+        <v>0.51</v>
+      </c>
+      <c r="E10" s="1" t="str">
+        <f>results!C10</f>
+        <v>(0.43--0.60)</v>
+      </c>
+      <c r="F10" s="10" t="str">
+        <f>results!D10</f>
+        <v>&lt;0.001</v>
+      </c>
+      <c r="G10" s="1" t="str">
+        <f>results!E10</f>
+        <v>***</v>
+      </c>
+      <c r="H10" s="1" t="str">
+        <f>results!F10</f>
+        <v>0.43</v>
+      </c>
+      <c r="I10" s="1" t="str">
+        <f>results!G10</f>
+        <v>0.60</v>
+      </c>
+    </row>
+    <row r="11" spans="2:9" x14ac:dyDescent="0.15">
+      <c r="B11" s="1" t="str">
+        <f>results!A11</f>
+        <v>male</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>266</v>
+      </c>
+      <c r="D11" s="12" t="str">
+        <f>results!B11</f>
+        <v>1.02</v>
+      </c>
+      <c r="E11" s="6" t="str">
+        <f>results!C11</f>
+        <v>(0.94--1.12)</v>
+      </c>
+      <c r="F11" s="12" t="str">
+        <f>results!D11</f>
+        <v>0.592</v>
+      </c>
+      <c r="G11" s="1" t="str">
+        <f>results!E11</f>
+        <v/>
+      </c>
+      <c r="H11" s="1" t="str">
+        <f>results!F11</f>
+        <v>0.94</v>
+      </c>
+      <c r="I11" s="1" t="str">
+        <f>results!G11</f>
+        <v>1.12</v>
+      </c>
+    </row>
+    <row r="12" spans="2:9" x14ac:dyDescent="0.15">
+      <c r="C12" s="23" t="s">
+        <v>267</v>
+      </c>
+      <c r="D12" s="24"/>
+      <c r="E12" s="25"/>
+      <c r="F12" s="24"/>
+    </row>
+    <row r="13" spans="2:9" x14ac:dyDescent="0.15">
+      <c r="C13" s="26" t="s">
+        <v>268</v>
+      </c>
+      <c r="D13" s="30" t="s">
+        <v>281</v>
+      </c>
+      <c r="E13" s="30"/>
+      <c r="F13" s="30"/>
+    </row>
+    <row r="14" spans="2:9" x14ac:dyDescent="0.15">
+      <c r="B14" s="1" t="str">
+        <f>results!A12</f>
+        <v>sepsis_dx1</v>
+      </c>
+      <c r="C14" s="26" t="s">
+        <v>269</v>
+      </c>
+      <c r="D14" s="24" t="str">
+        <f>results!B12</f>
+        <v>1.12</v>
+      </c>
+      <c r="E14" s="25" t="str">
+        <f>results!C12</f>
+        <v>(0.98--1.30)</v>
+      </c>
+      <c r="F14" s="24" t="str">
+        <f>results!D12</f>
+        <v>0.103</v>
+      </c>
+      <c r="G14" s="1" t="str">
+        <f>results!E12</f>
+        <v/>
+      </c>
+      <c r="H14" s="1" t="str">
+        <f>results!F12</f>
+        <v>0.98</v>
+      </c>
+      <c r="I14" s="1" t="str">
+        <f>results!G12</f>
+        <v>1.30</v>
+      </c>
+    </row>
+    <row r="15" spans="2:9" x14ac:dyDescent="0.15">
+      <c r="B15" s="1" t="str">
+        <f>results!A13</f>
+        <v>sepsis_dx2</v>
+      </c>
+      <c r="C15" s="26" t="s">
+        <v>270</v>
+      </c>
+      <c r="D15" s="24" t="str">
+        <f>results!B13</f>
+        <v>1.11</v>
+      </c>
+      <c r="E15" s="25" t="str">
+        <f>results!C13</f>
+        <v>(0.92--1.34)</v>
+      </c>
+      <c r="F15" s="24" t="str">
+        <f>results!D13</f>
+        <v>0.262</v>
+      </c>
+      <c r="G15" s="1" t="str">
+        <f>results!E13</f>
+        <v/>
+      </c>
+      <c r="H15" s="1" t="str">
+        <f>results!F13</f>
+        <v>0.92</v>
+      </c>
+      <c r="I15" s="1" t="str">
+        <f>results!G13</f>
+        <v>1.34</v>
+      </c>
+    </row>
+    <row r="16" spans="2:9" x14ac:dyDescent="0.15">
+      <c r="B16" s="1" t="str">
+        <f>results!A14</f>
+        <v>sepsis_dx3</v>
+      </c>
+      <c r="C16" s="26" t="s">
+        <v>271</v>
+      </c>
+      <c r="D16" s="24" t="str">
+        <f>results!B14</f>
+        <v>1.37</v>
+      </c>
+      <c r="E16" s="25" t="str">
+        <f>results!C14</f>
+        <v>(1.18--1.59)</v>
+      </c>
+      <c r="F16" s="24" t="str">
+        <f>results!D14</f>
+        <v>&lt;0.001</v>
+      </c>
+      <c r="G16" s="1" t="str">
+        <f>results!E14</f>
+        <v>***</v>
+      </c>
+      <c r="H16" s="1" t="str">
+        <f>results!F14</f>
+        <v>1.18</v>
+      </c>
+      <c r="I16" s="1" t="str">
+        <f>results!G14</f>
+        <v>1.59</v>
+      </c>
+    </row>
+    <row r="17" spans="2:9" x14ac:dyDescent="0.15">
+      <c r="B17" s="1" t="str">
+        <f>results!A15</f>
+        <v>sepsis_dx4</v>
+      </c>
+      <c r="C17" s="26" t="s">
+        <v>272</v>
+      </c>
+      <c r="D17" s="24" t="str">
+        <f>results!B15</f>
+        <v>1.25</v>
+      </c>
+      <c r="E17" s="25" t="str">
+        <f>results!C15</f>
+        <v>(1.12--1.40)</v>
+      </c>
+      <c r="F17" s="24" t="str">
+        <f>results!D15</f>
+        <v>&lt;0.001</v>
+      </c>
+      <c r="G17" s="1" t="str">
+        <f>results!E15</f>
+        <v>***</v>
+      </c>
+      <c r="H17" s="1" t="str">
+        <f>results!F15</f>
+        <v>1.12</v>
+      </c>
+      <c r="I17" s="1" t="str">
+        <f>results!G15</f>
+        <v>1.40</v>
+      </c>
+    </row>
+    <row r="18" spans="2:9" x14ac:dyDescent="0.15">
+      <c r="B18" s="1" t="str">
+        <f>results!A16</f>
+        <v>osupp2</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>273</v>
+      </c>
+      <c r="D18" s="12" t="str">
+        <f>results!B16</f>
+        <v>1.83</v>
+      </c>
+      <c r="E18" s="6" t="str">
+        <f>results!C16</f>
+        <v>(1.55--2.16)</v>
+      </c>
+      <c r="F18" s="12" t="str">
+        <f>results!D16</f>
+        <v>&lt;0.001</v>
+      </c>
+      <c r="G18" s="1" t="str">
+        <f>results!E16</f>
+        <v>***</v>
+      </c>
+      <c r="H18" s="1" t="str">
+        <f>results!F16</f>
+        <v>1.55</v>
+      </c>
+      <c r="I18" s="1" t="str">
+        <f>results!G16</f>
+        <v>2.16</v>
+      </c>
+    </row>
+    <row r="19" spans="2:9" x14ac:dyDescent="0.15">
+      <c r="B19" s="1" t="str">
+        <f>results!A17</f>
+        <v>icnarc_score</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>274</v>
+      </c>
+      <c r="D19" s="10" t="str">
+        <f>results!B17</f>
+        <v>1.07</v>
+      </c>
+      <c r="E19" s="1" t="str">
+        <f>results!C17</f>
+        <v>(1.06--1.08)</v>
+      </c>
+      <c r="F19" s="10" t="str">
+        <f>results!D17</f>
+        <v>&lt;0.001</v>
+      </c>
+      <c r="G19" s="1" t="str">
+        <f>results!E17</f>
+        <v>***</v>
+      </c>
+      <c r="H19" s="1" t="str">
+        <f>results!F17</f>
+        <v>1.06</v>
+      </c>
+      <c r="I19" s="1" t="str">
+        <f>results!G17</f>
+        <v>1.08</v>
+      </c>
+    </row>
+    <row r="20" spans="2:9" x14ac:dyDescent="0.15">
+      <c r="B20" s="1" t="str">
+        <f>results!A18</f>
+        <v>periarrest</v>
+      </c>
+      <c r="C20" s="20" t="s">
+        <v>275</v>
+      </c>
+      <c r="D20" s="21" t="str">
+        <f>results!B18</f>
+        <v>6.32</v>
+      </c>
+      <c r="E20" s="22" t="str">
+        <f>results!C18</f>
+        <v>(5.18--7.70)</v>
+      </c>
+      <c r="F20" s="21" t="str">
+        <f>results!D18</f>
+        <v>&lt;0.001</v>
+      </c>
+      <c r="G20" s="1" t="str">
+        <f>results!E18</f>
+        <v>***</v>
+      </c>
+      <c r="H20" s="1" t="str">
+        <f>results!F18</f>
+        <v>5.18</v>
+      </c>
+      <c r="I20" s="1" t="str">
+        <f>results!G18</f>
+        <v>7.70</v>
+      </c>
+    </row>
+    <row r="21" spans="2:9" s="25" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="C21" s="31"/>
+      <c r="D21" s="32"/>
+      <c r="E21" s="33"/>
+      <c r="F21" s="32"/>
+    </row>
+    <row r="22" spans="2:9" x14ac:dyDescent="0.15">
+      <c r="C22" s="2" t="s">
         <v>253</v>
       </c>
-      <c r="E6" s="13"/>
-    </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.15">
-      <c r="B7" s="1" t="str">
+      <c r="E22" s="13"/>
+    </row>
+    <row r="23" spans="2:9" x14ac:dyDescent="0.15">
+      <c r="B23" s="1" t="str">
         <f>results!A3</f>
         <v>out_of_hours</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C23" s="3" t="s">
         <v>254</v>
       </c>
-      <c r="D7" s="10" t="str">
+      <c r="D23" s="10" t="str">
         <f>results!B3</f>
         <v>1.47</v>
       </c>
-      <c r="E7" s="1" t="str">
+      <c r="E23" s="1" t="str">
         <f>results!C3</f>
         <v>(1.33--1.61)</v>
       </c>
-      <c r="F7" s="10" t="str">
+      <c r="F23" s="10" t="str">
         <f>results!D3</f>
         <v>&lt;0.001</v>
       </c>
-      <c r="G7" s="1" t="str">
+      <c r="G23" s="1" t="str">
         <f>results!E3</f>
         <v>***</v>
       </c>
-      <c r="H7" s="1" t="str">
+      <c r="H23" s="1" t="str">
         <f>results!F3</f>
         <v>1.33</v>
       </c>
-      <c r="I7" s="1" t="str">
+      <c r="I23" s="1" t="str">
         <f>results!G3</f>
         <v>1.61</v>
       </c>
     </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.15">
-      <c r="B8" s="1" t="str">
+    <row r="24" spans="2:9" x14ac:dyDescent="0.15">
+      <c r="B24" s="1" t="str">
         <f>results!A4</f>
         <v>weekend</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="C24" s="7" t="s">
         <v>255</v>
       </c>
-      <c r="D8" s="12" t="str">
+      <c r="D24" s="12" t="str">
         <f>results!B4</f>
         <v>1.15</v>
       </c>
-      <c r="E8" s="6" t="str">
+      <c r="E24" s="6" t="str">
         <f>results!C4</f>
         <v>(1.04--1.27)</v>
       </c>
-      <c r="F8" s="12" t="str">
+      <c r="F24" s="12" t="str">
         <f>results!D4</f>
         <v>0.006</v>
       </c>
-      <c r="G8" s="1" t="str">
+      <c r="G24" s="1" t="str">
         <f>results!E4</f>
         <v>**</v>
       </c>
-      <c r="H8" s="1" t="str">
+      <c r="H24" s="1" t="str">
         <f>results!F4</f>
         <v>1.04</v>
       </c>
-      <c r="I8" s="1" t="str">
+      <c r="I24" s="1" t="str">
         <f>results!G4</f>
         <v>1.27</v>
       </c>
     </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.15">
-      <c r="B9" s="1" t="str">
+    <row r="25" spans="2:9" x14ac:dyDescent="0.15">
+      <c r="B25" s="1" t="str">
         <f>results!A5</f>
         <v>winter</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C25" s="3" t="s">
         <v>256</v>
       </c>
-      <c r="D9" s="10" t="str">
+      <c r="D25" s="10" t="str">
         <f>results!B5</f>
         <v>1.19</v>
       </c>
-      <c r="E9" s="1" t="str">
+      <c r="E25" s="1" t="str">
         <f>results!C5</f>
         <v>(1.07--1.33)</v>
       </c>
-      <c r="F9" s="10" t="str">
+      <c r="F25" s="10" t="str">
         <f>results!D5</f>
         <v>0.002</v>
       </c>
-      <c r="G9" s="1" t="str">
+      <c r="G25" s="1" t="str">
         <f>results!E5</f>
         <v>**</v>
       </c>
-      <c r="H9" s="1" t="str">
+      <c r="H25" s="1" t="str">
         <f>results!F5</f>
         <v>1.07</v>
       </c>
-      <c r="I9" s="1" t="str">
+      <c r="I25" s="1" t="str">
         <f>results!G5</f>
         <v>1.33</v>
       </c>
     </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.15">
-      <c r="C10" s="5" t="s">
+    <row r="26" spans="2:9" x14ac:dyDescent="0.15">
+      <c r="C26" s="5" t="s">
         <v>260</v>
       </c>
-      <c r="D10" s="12"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="12"/>
-    </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.15">
-      <c r="C11" s="7" t="s">
+      <c r="D26" s="12"/>
+      <c r="E26" s="6"/>
+      <c r="F26" s="12"/>
+    </row>
+    <row r="27" spans="2:9" x14ac:dyDescent="0.15">
+      <c r="C27" s="7" t="s">
         <v>257</v>
       </c>
-      <c r="D11" s="22" t="s">
+      <c r="D27" s="28" t="s">
         <v>281</v>
       </c>
-      <c r="E11" s="22"/>
-      <c r="F11" s="22"/>
-    </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.15">
-      <c r="B12" s="1" t="str">
+      <c r="E27" s="28"/>
+      <c r="F27" s="28"/>
+    </row>
+    <row r="28" spans="2:9" x14ac:dyDescent="0.15">
+      <c r="B28" s="1" t="str">
         <f>results!A6</f>
         <v>room_cmp2[-5, 1)</v>
       </c>
-      <c r="C12" s="7" t="s">
+      <c r="C28" s="7" t="s">
         <v>258</v>
       </c>
-      <c r="D12" s="12" t="str">
+      <c r="D28" s="12" t="str">
+        <f>results!B7</f>
+        <v>0.89</v>
+      </c>
+      <c r="E28" s="12" t="str">
+        <f>results!C7</f>
+        <v>(0.79--1.00)</v>
+      </c>
+      <c r="F28" s="12" t="str">
+        <f>results!D7</f>
+        <v>0.055</v>
+      </c>
+      <c r="G28" s="1" t="str">
+        <f>results!E6</f>
+        <v>**</v>
+      </c>
+      <c r="H28" s="1" t="str">
+        <f>results!F6</f>
+        <v>0.59</v>
+      </c>
+      <c r="I28" s="1" t="str">
+        <f>results!G6</f>
+        <v>0.88</v>
+      </c>
+    </row>
+    <row r="29" spans="2:9" x14ac:dyDescent="0.15">
+      <c r="B29" s="1" t="str">
+        <f>results!A7</f>
+        <v>room_cmp2[ 1, 3)</v>
+      </c>
+      <c r="C29" s="7" t="s">
+        <v>259</v>
+      </c>
+      <c r="D29" s="12" t="str">
         <f>results!B6</f>
         <v>0.72</v>
       </c>
-      <c r="E12" s="6" t="str">
+      <c r="E29" s="12" t="str">
         <f>results!C6</f>
         <v>(0.59--0.88)</v>
       </c>
-      <c r="F12" s="12" t="str">
+      <c r="F29" s="12" t="str">
         <f>results!D6</f>
         <v>0.001</v>
       </c>
-      <c r="G12" s="1" t="str">
-        <f>results!E6</f>
-        <v>**</v>
-      </c>
-      <c r="H12" s="1" t="str">
-        <f>results!F6</f>
-        <v>0.59</v>
-      </c>
-      <c r="I12" s="1" t="str">
-        <f>results!G6</f>
-        <v>0.88</v>
-      </c>
-    </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.15">
-      <c r="B13" s="1" t="str">
-        <f>results!A7</f>
-        <v>room_cmp2[ 1, 3)</v>
-      </c>
-      <c r="C13" s="7" t="s">
-        <v>259</v>
-      </c>
-      <c r="D13" s="12" t="str">
-        <f>results!B7</f>
-        <v>0.89</v>
-      </c>
-      <c r="E13" s="6" t="str">
-        <f>results!C7</f>
-        <v>(0.79--1.00)</v>
-      </c>
-      <c r="F13" s="12" t="str">
-        <f>results!D7</f>
-        <v>0.055</v>
-      </c>
-      <c r="G13" s="1" t="str">
+      <c r="G29" s="1" t="str">
         <f>results!E7</f>
         <v/>
       </c>
-      <c r="H13" s="1" t="str">
+      <c r="H29" s="1" t="str">
         <f>results!F7</f>
         <v>0.79</v>
       </c>
-      <c r="I13" s="1" t="str">
+      <c r="I29" s="1" t="str">
         <f>results!G7</f>
         <v>1.00</v>
       </c>
     </row>
-    <row r="14" spans="2:9" x14ac:dyDescent="0.15">
-      <c r="C14" s="4" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="15" spans="2:9" x14ac:dyDescent="0.15">
-      <c r="C15" s="3" t="s">
-        <v>261</v>
-      </c>
-      <c r="D15" s="21" t="s">
-        <v>281</v>
-      </c>
-      <c r="E15" s="21"/>
-      <c r="F15" s="21"/>
-    </row>
-    <row r="16" spans="2:9" x14ac:dyDescent="0.15">
-      <c r="B16" s="1" t="str">
-        <f>results!A8</f>
-        <v>age_k1</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>262</v>
-      </c>
-      <c r="D16" s="10" t="str">
-        <f>results!B8</f>
-        <v>0.89</v>
-      </c>
-      <c r="E16" s="1" t="str">
-        <f>results!C8</f>
-        <v>(0.76--1.04)</v>
-      </c>
-      <c r="F16" s="10" t="str">
-        <f>results!D8</f>
-        <v>0.152</v>
-      </c>
-      <c r="G16" s="1" t="str">
-        <f>results!E8</f>
-        <v/>
-      </c>
-      <c r="H16" s="1" t="str">
-        <f>results!F8</f>
-        <v>0.76</v>
-      </c>
-      <c r="I16" s="1" t="str">
-        <f>results!G8</f>
-        <v>1.04</v>
-      </c>
-    </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.15">
-      <c r="B17" s="1" t="str">
-        <f>results!A9</f>
-        <v>age_k2</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>263</v>
-      </c>
-      <c r="D17" s="10" t="str">
-        <f>results!B9</f>
-        <v>0.76</v>
-      </c>
-      <c r="E17" s="1" t="str">
-        <f>results!C9</f>
-        <v>(0.66--0.89)</v>
-      </c>
-      <c r="F17" s="10" t="str">
-        <f>results!D9</f>
-        <v>&lt;0.001</v>
-      </c>
-      <c r="G17" s="1" t="str">
-        <f>results!E9</f>
-        <v>***</v>
-      </c>
-      <c r="H17" s="1" t="str">
-        <f>results!F9</f>
-        <v>0.66</v>
-      </c>
-      <c r="I17" s="1" t="str">
-        <f>results!G9</f>
-        <v>0.89</v>
-      </c>
-    </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.15">
-      <c r="B18" s="1" t="str">
-        <f>results!A10</f>
-        <v>age_k3</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>264</v>
-      </c>
-      <c r="D18" s="10" t="str">
-        <f>results!B10</f>
-        <v>0.51</v>
-      </c>
-      <c r="E18" s="1" t="str">
-        <f>results!C10</f>
-        <v>(0.43--0.60)</v>
-      </c>
-      <c r="F18" s="10" t="str">
-        <f>results!D10</f>
-        <v>&lt;0.001</v>
-      </c>
-      <c r="G18" s="1" t="str">
-        <f>results!E10</f>
-        <v>***</v>
-      </c>
-      <c r="H18" s="1" t="str">
-        <f>results!F10</f>
-        <v>0.43</v>
-      </c>
-      <c r="I18" s="1" t="str">
-        <f>results!G10</f>
-        <v>0.60</v>
-      </c>
-    </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.15">
-      <c r="B19" s="1" t="str">
-        <f>results!A11</f>
-        <v>male</v>
-      </c>
-      <c r="C19" s="8" t="s">
-        <v>266</v>
-      </c>
-      <c r="D19" s="12" t="str">
-        <f>results!B11</f>
-        <v>1.02</v>
-      </c>
-      <c r="E19" s="6" t="str">
-        <f>results!C11</f>
-        <v>(0.94--1.12)</v>
-      </c>
-      <c r="F19" s="12" t="str">
-        <f>results!D11</f>
-        <v>0.592</v>
-      </c>
-      <c r="G19" s="1" t="str">
-        <f>results!E11</f>
-        <v/>
-      </c>
-      <c r="H19" s="1" t="str">
-        <f>results!F11</f>
-        <v>0.94</v>
-      </c>
-      <c r="I19" s="1" t="str">
-        <f>results!G11</f>
-        <v>1.12</v>
-      </c>
-    </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.15">
-      <c r="C20" s="26" t="s">
-        <v>267</v>
-      </c>
-      <c r="D20" s="27"/>
-      <c r="E20" s="28"/>
-      <c r="F20" s="27"/>
-    </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.15">
-      <c r="C21" s="29" t="s">
-        <v>268</v>
-      </c>
-      <c r="D21" s="30" t="s">
-        <v>281</v>
-      </c>
-      <c r="E21" s="30"/>
-      <c r="F21" s="30"/>
-    </row>
-    <row r="22" spans="2:9" x14ac:dyDescent="0.15">
-      <c r="B22" s="1" t="str">
-        <f>results!A12</f>
-        <v>sepsis_dx1</v>
-      </c>
-      <c r="C22" s="29" t="s">
-        <v>269</v>
-      </c>
-      <c r="D22" s="27" t="str">
-        <f>results!B12</f>
-        <v>1.12</v>
-      </c>
-      <c r="E22" s="28" t="str">
-        <f>results!C12</f>
-        <v>(0.98--1.30)</v>
-      </c>
-      <c r="F22" s="27" t="str">
-        <f>results!D12</f>
-        <v>0.103</v>
-      </c>
-      <c r="G22" s="1" t="str">
-        <f>results!E12</f>
-        <v/>
-      </c>
-      <c r="H22" s="1" t="str">
-        <f>results!F12</f>
-        <v>0.98</v>
-      </c>
-      <c r="I22" s="1" t="str">
-        <f>results!G12</f>
-        <v>1.30</v>
-      </c>
-    </row>
-    <row r="23" spans="2:9" x14ac:dyDescent="0.15">
-      <c r="B23" s="1" t="str">
-        <f>results!A13</f>
-        <v>sepsis_dx2</v>
-      </c>
-      <c r="C23" s="29" t="s">
-        <v>270</v>
-      </c>
-      <c r="D23" s="27" t="str">
-        <f>results!B13</f>
-        <v>1.11</v>
-      </c>
-      <c r="E23" s="28" t="str">
-        <f>results!C13</f>
-        <v>(0.92--1.34)</v>
-      </c>
-      <c r="F23" s="27" t="str">
-        <f>results!D13</f>
-        <v>0.262</v>
-      </c>
-      <c r="G23" s="1" t="str">
-        <f>results!E13</f>
-        <v/>
-      </c>
-      <c r="H23" s="1" t="str">
-        <f>results!F13</f>
-        <v>0.92</v>
-      </c>
-      <c r="I23" s="1" t="str">
-        <f>results!G13</f>
-        <v>1.34</v>
-      </c>
-    </row>
-    <row r="24" spans="2:9" x14ac:dyDescent="0.15">
-      <c r="B24" s="1" t="str">
-        <f>results!A14</f>
-        <v>sepsis_dx3</v>
-      </c>
-      <c r="C24" s="29" t="s">
-        <v>271</v>
-      </c>
-      <c r="D24" s="27" t="str">
-        <f>results!B14</f>
-        <v>1.37</v>
-      </c>
-      <c r="E24" s="28" t="str">
-        <f>results!C14</f>
-        <v>(1.18--1.59)</v>
-      </c>
-      <c r="F24" s="27" t="str">
-        <f>results!D14</f>
-        <v>&lt;0.001</v>
-      </c>
-      <c r="G24" s="1" t="str">
-        <f>results!E14</f>
-        <v>***</v>
-      </c>
-      <c r="H24" s="1" t="str">
-        <f>results!F14</f>
-        <v>1.18</v>
-      </c>
-      <c r="I24" s="1" t="str">
-        <f>results!G14</f>
-        <v>1.59</v>
-      </c>
-    </row>
-    <row r="25" spans="2:9" x14ac:dyDescent="0.15">
-      <c r="B25" s="1" t="str">
-        <f>results!A15</f>
-        <v>sepsis_dx4</v>
-      </c>
-      <c r="C25" s="29" t="s">
-        <v>272</v>
-      </c>
-      <c r="D25" s="27" t="str">
-        <f>results!B15</f>
-        <v>1.25</v>
-      </c>
-      <c r="E25" s="28" t="str">
-        <f>results!C15</f>
-        <v>(1.12--1.40)</v>
-      </c>
-      <c r="F25" s="27" t="str">
-        <f>results!D15</f>
-        <v>&lt;0.001</v>
-      </c>
-      <c r="G25" s="1" t="str">
-        <f>results!E15</f>
-        <v>***</v>
-      </c>
-      <c r="H25" s="1" t="str">
-        <f>results!F15</f>
-        <v>1.12</v>
-      </c>
-      <c r="I25" s="1" t="str">
-        <f>results!G15</f>
-        <v>1.40</v>
-      </c>
-    </row>
-    <row r="26" spans="2:9" x14ac:dyDescent="0.15">
-      <c r="B26" s="1" t="str">
-        <f>results!A16</f>
-        <v>osupp2</v>
-      </c>
-      <c r="C26" s="8" t="s">
-        <v>273</v>
-      </c>
-      <c r="D26" s="12" t="str">
-        <f>results!B16</f>
-        <v>1.83</v>
-      </c>
-      <c r="E26" s="6" t="str">
-        <f>results!C16</f>
-        <v>(1.55--2.16)</v>
-      </c>
-      <c r="F26" s="12" t="str">
-        <f>results!D16</f>
-        <v>&lt;0.001</v>
-      </c>
-      <c r="G26" s="1" t="str">
-        <f>results!E16</f>
-        <v>***</v>
-      </c>
-      <c r="H26" s="1" t="str">
-        <f>results!F16</f>
-        <v>1.55</v>
-      </c>
-      <c r="I26" s="1" t="str">
-        <f>results!G16</f>
-        <v>2.16</v>
-      </c>
-    </row>
-    <row r="27" spans="2:9" x14ac:dyDescent="0.15">
-      <c r="B27" s="1" t="str">
-        <f>results!A17</f>
-        <v>icnarc_score</v>
-      </c>
-      <c r="C27" s="4" t="s">
-        <v>274</v>
-      </c>
-      <c r="D27" s="10" t="str">
-        <f>results!B17</f>
-        <v>1.07</v>
-      </c>
-      <c r="E27" s="1" t="str">
-        <f>results!C17</f>
-        <v>(1.06--1.08)</v>
-      </c>
-      <c r="F27" s="10" t="str">
-        <f>results!D17</f>
-        <v>&lt;0.001</v>
-      </c>
-      <c r="G27" s="1" t="str">
-        <f>results!E17</f>
-        <v>***</v>
-      </c>
-      <c r="H27" s="1" t="str">
-        <f>results!F17</f>
-        <v>1.06</v>
-      </c>
-      <c r="I27" s="1" t="str">
-        <f>results!G17</f>
-        <v>1.08</v>
-      </c>
-    </row>
-    <row r="28" spans="2:9" x14ac:dyDescent="0.15">
-      <c r="B28" s="1" t="str">
-        <f>results!A18</f>
-        <v>periarrest</v>
-      </c>
-      <c r="C28" s="23" t="s">
-        <v>275</v>
-      </c>
-      <c r="D28" s="24" t="str">
-        <f>results!B18</f>
-        <v>6.32</v>
-      </c>
-      <c r="E28" s="25" t="str">
-        <f>results!C18</f>
-        <v>(5.18--7.70)</v>
-      </c>
-      <c r="F28" s="24" t="str">
-        <f>results!D18</f>
-        <v>&lt;0.001</v>
-      </c>
-      <c r="G28" s="1" t="str">
-        <f>results!E18</f>
-        <v>***</v>
-      </c>
-      <c r="H28" s="1" t="str">
-        <f>results!F18</f>
-        <v>5.18</v>
-      </c>
-      <c r="I28" s="1" t="str">
-        <f>results!G18</f>
-        <v>7.70</v>
-      </c>
-    </row>
-    <row r="29" spans="2:9" x14ac:dyDescent="0.15">
-      <c r="C29" s="15"/>
-      <c r="D29" s="16"/>
-      <c r="E29" s="17"/>
-      <c r="F29" s="16"/>
-    </row>
     <row r="30" spans="2:9" x14ac:dyDescent="0.15">
-      <c r="C30" s="6" t="s">
+      <c r="C30" s="15"/>
+      <c r="D30" s="16"/>
+      <c r="E30" s="17"/>
+      <c r="F30" s="16"/>
+    </row>
+    <row r="31" spans="2:9" x14ac:dyDescent="0.15">
+      <c r="C31" s="6" t="s">
         <v>280</v>
       </c>
-      <c r="D30" s="12"/>
-      <c r="E30" s="6"/>
-      <c r="F30" s="12"/>
-    </row>
-    <row r="31" spans="2:9" x14ac:dyDescent="0.15">
-      <c r="C31" s="18" t="s">
+      <c r="D31" s="12"/>
+      <c r="E31" s="6"/>
+      <c r="F31" s="12"/>
+    </row>
+    <row r="32" spans="2:9" x14ac:dyDescent="0.15">
+      <c r="C32" s="18" t="s">
         <v>279</v>
       </c>
-      <c r="D31" s="19">
+      <c r="D32" s="19">
         <f>VALUE(boot!B2)</f>
         <v>2.1055545046014399</v>
       </c>
-      <c r="E31" s="18" t="str">
+      <c r="E32" s="18" t="str">
         <f>CONCATENATE("(",ROUND(VALUE(boot!C2),2),"--",ROUND(VALUE(boot!D2),2),")")</f>
         <v>(1.81--2.42)</v>
       </c>
-      <c r="F31" s="18"/>
+      <c r="F32" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="D5:E5"/>
-    <mergeCell ref="D11:F11"/>
-    <mergeCell ref="D15:F15"/>
-    <mergeCell ref="D21:F21"/>
+    <mergeCell ref="D27:F27"/>
+    <mergeCell ref="D7:F7"/>
+    <mergeCell ref="D13:F13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>